<commit_message>
Major update. Schedule, New Parameters.
Schedule - schedule on month calendar days and working days now available.
New parameters for debugging, termination.
Emailing system works now, only needs to be configured (SMTP / Outlook)
</commit_message>
<xml_diff>
--- a/Tests/Test Parameters.xlsx
+++ b/Tests/Test Parameters.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Power Refresh\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-Refresh\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7248F72-4980-4CD1-9C2A-B8750230483C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -432,7 +433,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:C3"/>
   <sheetViews>
@@ -440,21 +441,21 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>

</xml_diff>